<commit_message>
Report - edit FCM Instance
</commit_message>
<xml_diff>
--- a/REPORT.xlsx
+++ b/REPORT.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects (PHP)\IDareYou\IDareYou\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ichallengeyou\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4131C03E-65C6-41E3-9994-BC7144C3EC22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="To Do" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>When creating new challenge, it is not available in my challenges list</t>
   </si>
@@ -62,12 +61,24 @@
   </si>
   <si>
     <t>Get Paypal and fcm settings from database</t>
+  </si>
+  <si>
+    <t>Already Done</t>
+  </si>
+  <si>
+    <t>On Submit Challenge</t>
+  </si>
+  <si>
+    <t>CHALLENGE_SCREEN</t>
+  </si>
+  <si>
+    <t>Donator - $user_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -103,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -113,6 +124,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -393,20 +410,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="76.42578125" customWidth="1"/>
+    <col min="1" max="1" width="76.42578125" style="5" customWidth="1"/>
     <col min="2" max="2" width="14.140625" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -414,39 +432,45 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -457,11 +481,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E30CF73-4069-4118-97A8-BE452E42E097}">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,7 +495,7 @@
     <col min="3" max="3" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -482,6 +506,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Voter can cote only one challenger
</commit_message>
<xml_diff>
--- a/REPORT.xlsx
+++ b/REPORT.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr showObjects="none" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ichallengeyou\"/>
@@ -16,6 +16,7 @@
     <sheet name="Notifications" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -117,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -132,6 +133,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -414,20 +418,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="76.42578125" style="5" customWidth="1"/>
     <col min="2" max="2" width="14.140625" style="3" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -435,7 +439,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -443,7 +447,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -451,7 +455,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -459,7 +463,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -467,7 +471,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -475,18 +479,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add pagination in challenge submitted users list
</commit_message>
<xml_diff>
--- a/REPORT.xlsx
+++ b/REPORT.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>When creating new challenge, it is not available in my challenges list</t>
   </si>
@@ -448,7 +448,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9:XFD9"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,6 +525,9 @@
     <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>15</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>

</xml_diff>

<commit_message>
bids,submitedList Btns keys & category Filter
</commit_message>
<xml_diff>
--- a/REPORT.xlsx
+++ b/REPORT.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>When creating new challenge, it is not available in my challenges list</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Add pagination in challenge submitted users list</t>
   </si>
   <si>
-    <t>add review button key in challenge detail api</t>
-  </si>
-  <si>
     <t>add bid button key in challenge detail api</t>
   </si>
   <si>
@@ -106,6 +103,9 @@
   </si>
   <si>
     <t>Add category filter in challenges get list api</t>
+  </si>
+  <si>
+    <t>add submited-challenge-users-list-button key in challenge detail api</t>
   </si>
 </sst>
 </file>
@@ -147,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -163,6 +163,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -447,8 +450,8 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,7 +463,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
@@ -534,47 +537,56 @@
     </row>
     <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>16</v>
+        <v>26</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -614,7 +626,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
convert notifications to polymorphism & buttons keys conditions
</commit_message>
<xml_diff>
--- a/REPORT.xlsx
+++ b/REPORT.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>When creating new challenge, it is not available in my challenges list</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>add submited-challenge-users-list-button key in challenge detail api</t>
+  </si>
+  <si>
+    <t>++</t>
+  </si>
+  <si>
+    <t>Bidding API</t>
   </si>
 </sst>
 </file>
@@ -147,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -165,6 +171,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -447,11 +456,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,29 +572,40 @@
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="B13" s="6" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>19</v>
+        <v>28</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BID API Completed - biding & Listing
</commit_message>
<xml_diff>
--- a/REPORT.xlsx
+++ b/REPORT.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>When creating new challenge, it is not available in my challenges list</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>add submited-challenge-users-list-button key in challenge detail api</t>
-  </si>
-  <si>
-    <t>++</t>
   </si>
   <si>
     <t>Bidding API</t>
@@ -460,7 +457,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,10 +575,10 @@
     </row>
     <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
doantor cant accept and submit challenge
</commit_message>
<xml_diff>
--- a/REPORT.xlsx
+++ b/REPORT.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
   <si>
     <t>When creating new challenge, it is not available in my challenges list</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>ASK_RESULT_DIALOG</t>
+  </si>
+  <si>
+    <t>Challenge ID</t>
   </si>
 </sst>
 </file>
@@ -648,7 +651,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,6 +713,9 @@
       </c>
       <c r="C4" s="4" t="s">
         <v>34</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Message[premium] ,fixed record-Filter , Complete Edit Challenge in WEB
</commit_message>
<xml_diff>
--- a/REPORT.xlsx
+++ b/REPORT.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" tabRatio="438" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" tabRatio="438"/>
   </bookViews>
   <sheets>
     <sheet name="To Do" sheetId="1" r:id="rId1"/>
     <sheet name="Notifications" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>When creating new challenge, it is not available in my challenges list</t>
   </si>
@@ -486,9 +487,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,7 +601,7 @@
       <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -615,6 +616,9 @@
     <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>18</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -647,7 +651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
on settings edit check the type of setting then show appropriate input type field
</commit_message>
<xml_diff>
--- a/REPORT.xlsx
+++ b/REPORT.xlsx
@@ -16,7 +16,6 @@
     <sheet name="Notifications" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
   <si>
     <t>When creating new challenge, it is not available in my challenges list</t>
   </si>
@@ -59,9 +58,6 @@
   </si>
   <si>
     <t>Get Paypal and fcm settings from database</t>
-  </si>
-  <si>
-    <t>Already Done</t>
   </si>
   <si>
     <t>On Submit Challenge</t>
@@ -487,9 +483,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +497,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
@@ -536,7 +532,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -549,7 +545,7 @@
     </row>
     <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
@@ -565,7 +561,7 @@
     </row>
     <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>6</v>
@@ -575,7 +571,7 @@
     </row>
     <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>6</v>
@@ -583,7 +579,7 @@
     </row>
     <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>6</v>
@@ -591,7 +587,7 @@
     </row>
     <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>6</v>
@@ -599,7 +595,7 @@
     </row>
     <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>6</v>
@@ -607,7 +603,7 @@
     </row>
     <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>6</v>
@@ -615,7 +611,7 @@
     </row>
     <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>6</v>
@@ -623,22 +619,34 @@
     </row>
     <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="B18" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>21</v>
+      <c r="B19" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -674,49 +682,49 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="C3" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="C4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
soft Delete in user Model
</commit_message>
<xml_diff>
--- a/REPORT.xlsx
+++ b/REPORT.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
   <si>
     <t>When creating new challenge, it is not available in my challenges list</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>User Soft Deletes</t>
+  </si>
+  <si>
+    <t>Payment Transaction in Create Challenge</t>
   </si>
 </sst>
 </file>
@@ -484,11 +487,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,6 +658,17 @@
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>34</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in admin web
</commit_message>
<xml_diff>
--- a/REPORT.xlsx
+++ b/REPORT.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
   <si>
     <t>When creating new challenge, it is not available in my challenges list</t>
   </si>
@@ -136,6 +136,21 @@
   </si>
   <si>
     <t>Transaction for admin web</t>
+  </si>
+  <si>
+    <t>Chache on listing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notification Against Transaction </t>
+  </si>
+  <si>
+    <t>Notifcication Against Reaction on challenge</t>
+  </si>
+  <si>
+    <t>Donate within time</t>
+  </si>
+  <si>
+    <t>post submit challenge</t>
   </si>
 </sst>
 </file>
@@ -490,11 +505,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21:B22"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,6 +695,34 @@
       </c>
       <c r="B22" s="3" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
store cache with static key , description in getList & acceptor and submitor in admin web
</commit_message>
<xml_diff>
--- a/REPORT.xlsx
+++ b/REPORT.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
   <si>
     <t>When creating new challenge, it is not available in my challenges list</t>
   </si>
@@ -150,7 +150,16 @@
     <t>Donate within time</t>
   </si>
   <si>
-    <t>post submit challenge</t>
+    <t>post submit challenge Test</t>
+  </si>
+  <si>
+    <t>++</t>
+  </si>
+  <si>
+    <t>add discription when sharing</t>
+  </si>
+  <si>
+    <t>show description in getList</t>
   </si>
 </sst>
 </file>
@@ -505,11 +514,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,11 +715,17 @@
       <c r="A24" s="5" t="s">
         <v>38</v>
       </c>
+      <c r="B24" s="6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>39</v>
       </c>
+      <c r="B25" s="6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
@@ -723,6 +738,19 @@
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>41</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add click_action of submit challenge
</commit_message>
<xml_diff>
--- a/REPORT.xlsx
+++ b/REPORT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" tabRatio="438"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" tabRatio="438" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="To Do" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="60">
   <si>
     <t>When creating new challenge, it is not available in my challenges list</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Bidding API</t>
   </si>
   <si>
-    <t xml:space="preserve">On Vote </t>
-  </si>
-  <si>
     <t>Challenger</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>Accepted Challenge ID</t>
   </si>
   <si>
-    <t>On Result</t>
-  </si>
-  <si>
     <t>Candidate</t>
   </si>
   <si>
@@ -160,13 +154,64 @@
   </si>
   <si>
     <t>show description in getList</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>On Load Balanace</t>
+  </si>
+  <si>
+    <t>to Admin</t>
+  </si>
+  <si>
+    <t>ADMIN_NOTIFICATION</t>
+  </si>
+  <si>
+    <t>On Create Challage</t>
+  </si>
+  <si>
+    <t>User ID</t>
+  </si>
+  <si>
+    <t>Challenge ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On Donate </t>
+  </si>
+  <si>
+    <t>to Admin, Creater</t>
+  </si>
+  <si>
+    <t>On Withdraw</t>
+  </si>
+  <si>
+    <t>On Miscellaneous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On Win </t>
+  </si>
+  <si>
+    <t>To Donator, Creator, Submitor &amp; Winner</t>
+  </si>
+  <si>
+    <t>CHALLENGE_DETAIL_SCREEN</t>
+  </si>
+  <si>
+    <t>On Second Vote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On First Vote </t>
+  </si>
+  <si>
+    <t>SUBMITED_CHALLENGE_LIST_SCREEN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +221,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -208,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -232,6 +284,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -516,9 +571,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,7 +739,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>6</v>
@@ -692,7 +747,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>6</v>
@@ -700,7 +755,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>6</v>
@@ -708,28 +763,31 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>6</v>
@@ -737,7 +795,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>6</v>
@@ -745,12 +803,18 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -763,15 +827,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.5703125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -786,7 +850,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -797,46 +861,124 @@
         <v>16</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="C3" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="11" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
on First Vote Notification
</commit_message>
<xml_diff>
--- a/REPORT.xlsx
+++ b/REPORT.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="61">
   <si>
     <t>When creating new challenge, it is not available in my challenges list</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>SUBMITED_CHALLENGE_LIST_SCREEN</t>
+  </si>
+  <si>
+    <t>migrate data_id in notifications table</t>
   </si>
 </sst>
 </file>
@@ -569,11 +572,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -817,6 +820,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -825,10 +836,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,9 +848,10 @@
     <col min="2" max="2" width="43.28515625" style="4" customWidth="1"/>
     <col min="3" max="3" width="45.7109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -853,7 +865,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -866,8 +878,11 @@
       <c r="D2" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>58</v>
       </c>
@@ -881,7 +896,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>57</v>
       </c>
@@ -895,7 +910,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>44</v>
       </c>
@@ -909,7 +924,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -923,7 +938,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>52</v>
       </c>
@@ -937,7 +952,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>50</v>
       </c>
@@ -951,7 +966,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>47</v>
       </c>
@@ -965,7 +980,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>54</v>
       </c>
@@ -979,12 +994,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Notification against transaction implement Queues
</commit_message>
<xml_diff>
--- a/REPORT.xlsx
+++ b/REPORT.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="63">
   <si>
     <t>When creating new challenge, it is not available in my challenges list</t>
   </si>
@@ -180,9 +180,6 @@
     <t xml:space="preserve">On Donate </t>
   </si>
   <si>
-    <t>to Admin, Creater</t>
-  </si>
-  <si>
     <t>On Withdraw</t>
   </si>
   <si>
@@ -208,6 +205,15 @@
   </si>
   <si>
     <t>migrate data_id in notifications table</t>
+  </si>
+  <si>
+    <t>to Admin, Current User</t>
+  </si>
+  <si>
+    <t>Api</t>
+  </si>
+  <si>
+    <t>to Admin, Creater, Current User</t>
   </si>
 </sst>
 </file>
@@ -812,7 +818,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>6</v>
@@ -826,10 +832,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,7 +847,7 @@
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -855,7 +861,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -871,10 +877,13 @@
       <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>26</v>
@@ -888,10 +897,13 @@
       <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>29</v>
@@ -903,12 +915,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>46</v>
@@ -916,13 +928,19 @@
       <c r="D5" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>46</v>
@@ -930,13 +948,19 @@
       <c r="D6" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>46</v>
@@ -944,25 +968,34 @@
       <c r="D7" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>47</v>
       </c>
@@ -976,26 +1009,26 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="C10" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
on Win Notification for doantor creater submitors & Winner
</commit_message>
<xml_diff>
--- a/REPORT.xlsx
+++ b/REPORT.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="63">
   <si>
     <t>When creating new challenge, it is not available in my challenges list</t>
   </si>
@@ -835,7 +835,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,7 +1023,10 @@
         <v>49</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>40</v>
+        <v>6</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
correct message add -> $ and update report
</commit_message>
<xml_diff>
--- a/REPORT.xlsx
+++ b/REPORT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" tabRatio="438" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" tabRatio="438"/>
   </bookViews>
   <sheets>
     <sheet name="To Do" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="61">
   <si>
     <t>When creating new challenge, it is not available in my challenges list</t>
   </si>
@@ -147,16 +147,10 @@
     <t>post submit challenge Test</t>
   </si>
   <si>
-    <t>++</t>
-  </si>
-  <si>
     <t>add discription when sharing</t>
   </si>
   <si>
     <t>show description in getList</t>
-  </si>
-  <si>
-    <t>+</t>
   </si>
   <si>
     <t>On Load Balanace</t>
@@ -570,9 +564,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,7 +759,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -773,7 +767,7 @@
         <v>36</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -781,7 +775,7 @@
         <v>37</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -802,7 +796,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>6</v>
@@ -810,7 +804,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>6</v>
@@ -818,7 +812,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>6</v>
@@ -834,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,12 +872,12 @@
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>26</v>
@@ -898,12 +892,12 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>29</v>
@@ -917,116 +911,116 @@
     </row>
     <row r="5" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="E5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="E6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="E7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Vote exception , view submitChallengeDetail in web tbc
</commit_message>
<xml_diff>
--- a/REPORT.xlsx
+++ b/REPORT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" tabRatio="438"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" tabRatio="438" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="To Do" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="62">
   <si>
     <t>When creating new challenge, it is not available in my challenges list</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>show description in getList</t>
+  </si>
+  <si>
+    <t>+</t>
   </si>
   <si>
     <t>On Load Balanace</t>
@@ -564,9 +567,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,7 +762,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -812,7 +815,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>6</v>
@@ -828,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,12 +875,12 @@
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>26</v>
@@ -892,12 +895,12 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>29</v>
@@ -911,116 +914,116 @@
     </row>
     <row r="5" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="E8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="D9" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fix notification bug & complete isWinner from admin
</commit_message>
<xml_diff>
--- a/REPORT.xlsx
+++ b/REPORT.xlsx
@@ -114,9 +114,6 @@
     <t>Accepted Challenge ID</t>
   </si>
   <si>
-    <t>Candidate</t>
-  </si>
-  <si>
     <t>SUBMITED_CHALLENGE_DETAIL_SCREEN</t>
   </si>
   <si>
@@ -211,6 +208,9 @@
   </si>
   <si>
     <t>to Admin, Creater, Current User</t>
+  </si>
+  <si>
+    <t>Candidates</t>
   </si>
 </sst>
 </file>
@@ -735,7 +735,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>6</v>
@@ -743,7 +743,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>6</v>
@@ -751,7 +751,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>6</v>
@@ -759,15 +759,15 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>6</v>
@@ -775,7 +775,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>6</v>
@@ -783,7 +783,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>6</v>
@@ -791,7 +791,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>6</v>
@@ -799,7 +799,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>6</v>
@@ -807,7 +807,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>6</v>
@@ -815,7 +815,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>6</v>
@@ -832,7 +832,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,7 +866,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>28</v>
@@ -875,18 +875,18 @@
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>28</v>
@@ -895,18 +895,18 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>28</v>
@@ -914,116 +914,116 @@
     </row>
     <row r="5" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="D9" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="C10" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Winner Notification for admin web
</commit_message>
<xml_diff>
--- a/REPORT.xlsx
+++ b/REPORT.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="63">
   <si>
     <t>When creating new challenge, it is not available in my challenges list</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Send notification to user on vote on submitted challenge</t>
   </si>
   <si>
-    <t>Donator - Creator</t>
-  </si>
-  <si>
     <t>Create edit challenge page for admin web</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>Bidding API</t>
   </si>
   <si>
-    <t>Challenger</t>
-  </si>
-  <si>
     <t>data_id</t>
   </si>
   <si>
@@ -183,9 +177,6 @@
     <t xml:space="preserve">On Win </t>
   </si>
   <si>
-    <t>To Donator, Creator, Submitor &amp; Winner</t>
-  </si>
-  <si>
     <t>CHALLENGE_DETAIL_SCREEN</t>
   </si>
   <si>
@@ -211,6 +202,18 @@
   </si>
   <si>
     <t>Candidates</t>
+  </si>
+  <si>
+    <t>Donator - Creator - Admin</t>
+  </si>
+  <si>
+    <t>Challenger - Admin</t>
+  </si>
+  <si>
+    <t>Web</t>
+  </si>
+  <si>
+    <t>To Donator, Creator, Submitor ,Winner &amp; Admin</t>
   </si>
 </sst>
 </file>
@@ -581,7 +584,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
@@ -655,7 +658,7 @@
     </row>
     <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>6</v>
@@ -663,7 +666,7 @@
     </row>
     <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>6</v>
@@ -687,7 +690,7 @@
     </row>
     <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>6</v>
@@ -695,7 +698,7 @@
     </row>
     <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>6</v>
@@ -703,7 +706,7 @@
     </row>
     <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>6</v>
@@ -711,7 +714,7 @@
     </row>
     <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>6</v>
@@ -719,7 +722,7 @@
     </row>
     <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>6</v>
@@ -727,7 +730,7 @@
     </row>
     <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>6</v>
@@ -735,7 +738,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>6</v>
@@ -743,7 +746,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>6</v>
@@ -751,7 +754,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>6</v>
@@ -759,15 +762,15 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>6</v>
@@ -775,7 +778,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>6</v>
@@ -783,7 +786,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>6</v>
@@ -791,7 +794,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>6</v>
@@ -799,7 +802,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>6</v>
@@ -807,7 +810,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>6</v>
@@ -815,7 +818,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>6</v>
@@ -829,10 +832,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,7 +847,7 @@
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -855,190 +858,210 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="D4" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="C5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    </row>
+    <row r="6" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="B8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="D8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="8" t="s">
+      <c r="B9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="E9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="B10" s="4" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add $ , onCreateChallenge Notification is completed
</commit_message>
<xml_diff>
--- a/REPORT.xlsx
+++ b/REPORT.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="63">
   <si>
     <t>When creating new challenge, it is not available in my challenges list</t>
   </si>
@@ -150,9 +150,6 @@
     <t>On Load Balanace</t>
   </si>
   <si>
-    <t>to Admin</t>
-  </si>
-  <si>
     <t>ADMIN_NOTIFICATION</t>
   </si>
   <si>
@@ -214,6 +211,9 @@
   </si>
   <si>
     <t>To Donator, Creator, Submitor ,Winner &amp; Admin</t>
+  </si>
+  <si>
+    <t>to Challenge Owner, to Admin</t>
   </si>
 </sst>
 </file>
@@ -818,7 +818,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>6</v>
@@ -834,7 +834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -866,7 +866,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>27</v>
@@ -878,18 +878,18 @@
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>27</v>
@@ -901,24 +901,30 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>26</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -926,128 +932,137 @@
         <v>40</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="G5" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="G6" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="G7" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>42</v>
+        <v>62</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>49</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Tied result notification for admin wenb
</commit_message>
<xml_diff>
--- a/REPORT.xlsx
+++ b/REPORT.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="63">
   <si>
     <t>When creating new challenge, it is not available in my challenges list</t>
   </si>
@@ -111,9 +111,6 @@
     <t>SUBMITED_CHALLENGE_DETAIL_SCREEN</t>
   </si>
   <si>
-    <t>ASK_RESULT_DIALOG</t>
-  </si>
-  <si>
     <t>User Soft Deletes</t>
   </si>
   <si>
@@ -198,9 +195,6 @@
     <t>to Admin, Creater, Current User</t>
   </si>
   <si>
-    <t>Candidates</t>
-  </si>
-  <si>
     <t>Donator - Creator - Admin</t>
   </si>
   <si>
@@ -214,6 +208,12 @@
   </si>
   <si>
     <t>to Challenge Owner, to Admin</t>
+  </si>
+  <si>
+    <t>Candidates , Admin</t>
+  </si>
+  <si>
+    <t>ASK_RESULT_DIALOG, CHALLENGE_DETAIL_SCREEN</t>
   </si>
 </sst>
 </file>
@@ -738,7 +738,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>6</v>
@@ -746,7 +746,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>6</v>
@@ -754,7 +754,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>6</v>
@@ -762,15 +762,15 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>6</v>
@@ -778,7 +778,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>6</v>
@@ -786,7 +786,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>6</v>
@@ -794,7 +794,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>6</v>
@@ -802,7 +802,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>6</v>
@@ -810,7 +810,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>6</v>
@@ -818,7 +818,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>6</v>
@@ -835,7 +835,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,7 +866,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>27</v>
@@ -878,18 +878,18 @@
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>27</v>
@@ -901,21 +901,21 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>26</v>
@@ -924,145 +924,148 @@
         <v>6</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="D5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="G5" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="G6" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="G7" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
register comment Observer & refactor code
</commit_message>
<xml_diff>
--- a/REPORT.xlsx
+++ b/REPORT.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
   <si>
     <t>When creating new challenge, it is not available in my challenges list</t>
   </si>
@@ -192,9 +192,6 @@
     <t>to Admin, Creater, Current User</t>
   </si>
   <si>
-    <t>Donator - Creator - Admin</t>
-  </si>
-  <si>
     <t>Challenger - Admin</t>
   </si>
   <si>
@@ -214,6 +211,21 @@
   </si>
   <si>
     <t>ADMIN_NOTIFICATION , TRANSACTION_LIST</t>
+  </si>
+  <si>
+    <t>Donator - Creator - Admin - User</t>
+  </si>
+  <si>
+    <t>Notification Against Comment</t>
+  </si>
+  <si>
+    <t>++</t>
+  </si>
+  <si>
+    <t>Email Against Transaction</t>
+  </si>
+  <si>
+    <t>on Comments</t>
   </si>
 </sst>
 </file>
@@ -568,11 +580,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,6 +836,22 @@
         <v>6</v>
       </c>
     </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -834,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,7 +894,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>27</v>
@@ -881,7 +909,7 @@
         <v>53</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -889,7 +917,7 @@
         <v>49</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>27</v>
@@ -904,7 +932,7 @@
         <v>53</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -912,10 +940,10 @@
         <v>48</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>26</v>
@@ -927,7 +955,7 @@
         <v>53</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -938,7 +966,7 @@
         <v>52</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>41</v>
@@ -950,7 +978,7 @@
         <v>53</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -961,7 +989,7 @@
         <v>52</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>41</v>
@@ -973,7 +1001,7 @@
         <v>53</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -984,7 +1012,7 @@
         <v>52</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>41</v>
@@ -996,7 +1024,7 @@
         <v>53</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -1019,7 +1047,7 @@
         <v>53</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -1027,7 +1055,7 @@
         <v>46</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>50</v>
@@ -1042,7 +1070,7 @@
         <v>53</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -1050,7 +1078,7 @@
         <v>40</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>47</v>
@@ -1065,10 +1093,14 @@
         <v>53</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="12" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>